<commit_message>
Import data from excel file as string.
</commit_message>
<xml_diff>
--- a/Project_final_2022_2023/bin/Debug/net6.0-windows/Questions.xlsx
+++ b/Project_final_2022_2023/bin/Debug/net6.0-windows/Questions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4181db737fe83a3d/5o Εξάμηνο/Λογισμικό Διαχείρισης Μάθησης/Απαλλακτική Εργασία 2022/Project/project_final/Project_final_2022_2023/bin/Debug/net6.0-windows/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\project_final\Project_final_2022_2023\bin\Debug\net6.0-windows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="8_{ACD40CE2-1458-4080-9661-598329397260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{738930E7-5A8B-47B5-B526-73BC53C6DF89}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF18F6B-1B5E-4C47-B393-9A259EC4E471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9180" yWindow="4155" windowWidth="21600" windowHeight="11295" xr2:uid="{8DA8C0F3-3EB6-40DE-8DFC-E7A0383F4D3D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8DA8C0F3-3EB6-40DE-8DFC-E7A0383F4D3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Questions</t>
   </si>
@@ -117,19 +117,59 @@
   </si>
   <si>
     <t>rt</t>
+  </si>
+  <si>
+    <t>Βαλε στην θεση τα αντιστοιχα συμβολα ( + , - , x , / ) ωστε η πραξει να ειναι ορθη :</t>
+  </si>
+  <si>
+    <t>Βαλε στην θεση τα αντιστοιχα συμβολα ( &lt; , = , &gt; ) ωστε να ειναι ορθα:</t>
+  </si>
+  <si>
+    <t>Βαλε στην αυξουσα σειρα τους παρακατω αριθμους:</t>
+  </si>
+  <si>
+    <t>["1    2   = 3",
+"3    3   =  9",
+"10   2  =  5 ",
+"7     3  =  4"]</t>
+  </si>
+  <si>
+    <t>["+","x","/","-"]</t>
+  </si>
+  <si>
+    <t>["1      3",
+"5      2",
+"10    10",
+"3      9", 
+"7      3"]</t>
+  </si>
+  <si>
+    <t>["&lt;","&gt;","=","&lt;","&gt;"]</t>
+  </si>
+  <si>
+    <t>["1", " 4"," 3," 2","7"," 9","10","8","5","6"]</t>
+  </si>
+  <si>
+    <t>["1","2","3","4","5","6","7","8","9","10"]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -152,10 +192,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -473,20 +516,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2837E2A6-D3C0-44EE-8D08-D1968BD1F869}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="117" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" customWidth="1"/>
-    <col min="3" max="3" width="80.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="80.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,7 +543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -514,7 +557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -528,7 +571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -542,7 +585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -556,7 +599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -570,7 +613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -584,7 +627,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -598,7 +641,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -612,7 +655,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -626,12 +669,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -639,12 +682,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -658,7 +701,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -666,7 +709,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -674,23 +717,50 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="57.6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="B17" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="72" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="B18" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="B19" s="1">
         <v>6</v>
       </c>
+      <c r="C19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Clean and rebuild project. notes.txt and questions.xlsx updated.
</commit_message>
<xml_diff>
--- a/Project_final_2022_2023/bin/Debug/net6.0-windows/Questions.xlsx
+++ b/Project_final_2022_2023/bin/Debug/net6.0-windows/Questions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\project_final\Project_final_2022_2023\bin\Debug\net6.0-windows\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipigr-my.sharepoint.com/personal/p20004_unipi_gr/Documents/Logismiko_Diaxeirishs_Mathishs/Apallaktikh_ergasia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF18F6B-1B5E-4C47-B393-9A259EC4E471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{1B726E18-D274-41B2-BD47-1654DE0783A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AD14668-2AB5-4146-AE70-D0913955CCB2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8DA8C0F3-3EB6-40DE-8DFC-E7A0383F4D3D}"/>
+    <workbookView xWindow="38280" yWindow="-3375" windowWidth="29040" windowHeight="15720" xr2:uid="{8DA8C0F3-3EB6-40DE-8DFC-E7A0383F4D3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
-  <si>
-    <t>Questions</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>Type</t>
   </si>
@@ -50,107 +47,139 @@
     <t>Answers</t>
   </si>
   <si>
-    <t>["Σ" , "Λ"]</t>
-  </si>
-  <si>
     <t>Η Μαρία έχει 19 κάρτες και ο Μιχάλης 7. Για να έχει η Μαρία τον ίδιο αριθμό καρτών θα πρέπει να αφήσει 12 κάρτες κάτω.</t>
   </si>
   <si>
-    <t>Οι βαθμοί ενός μαθητή σε 6 μαθήματα ήταν 7,10,7,8,7,9. Ο μέσος όρος του θα είναι 8.</t>
-  </si>
-  <si>
-    <t>Μία παρέα 5 ατόμων μάζεψαν 65 κοχύλια και θέλουν να τα μοιραστούν εξίσου. Άρα το κάθε παιδί θα πάρει 13 κοχύλια.</t>
-  </si>
-  <si>
-    <t>Πως λέγεται η πράξη που πραγματοποιείται με το σύμβολο "x";</t>
-  </si>
-  <si>
-    <t>["Γινόμενο","Πολλαπλασιασμός","Η πράξη με το «x»","Μέθοδος των τριών"]</t>
-  </si>
-  <si>
-    <t>Πως γράφεται η πράξη που πραγματοποιείται με το σύμβολο "x";</t>
-  </si>
-  <si>
-    <t>["Πολαπλασιασμός","Πολλαπλασσιασμός","Πολλαπλασιασμός","Πολλαπλασειασμός"]</t>
-  </si>
-  <si>
     <t>Ποιο είναι το αποτέλεσμα της πράξης 6x34;</t>
   </si>
   <si>
-    <t>["200","204","198","104"]</t>
-  </si>
-  <si>
-    <t>Ποιο είναι το αποτέλεσμα της πράξης 48 ÷ 6;</t>
-  </si>
-  <si>
-    <t>[" 8,0","Δεν το έχουμε μάθει."," 8","Δεν έχει υπόλοιπο."]</t>
-  </si>
-  <si>
-    <t>1, 3, 4</t>
-  </si>
-  <si>
     <t>Ποια είναι τα πιθανά σύμβολα της διαίρεσης και του πολλαπλασιασμού, αντίστοιχα;</t>
   </si>
   <si>
-    <t>["÷ και x","/ και .","÷ και "," / και *"]</t>
-  </si>
-  <si>
-    <t>1, 4</t>
-  </si>
-  <si>
     <t>Ποιοι είναι οι διαιρέτες του 36;</t>
   </si>
   <si>
-    <t>["1 και 2"," 6 και 9","18 και 8","4 και 10"]</t>
-  </si>
-  <si>
-    <t>1, 2</t>
-  </si>
-  <si>
-    <t>[["Πυθαγόρειο","addition"],["Πρόσθεση","subtraction"],["Αφαίρεση","Θεώρημα"]]</t>
-  </si>
-  <si>
-    <t>[[2],[1],[],[3]]</t>
-  </si>
-  <si>
-    <t>Να αντιστοιχίσετε κάθε στοιχείο της στήλης Α με ένα στοιχείο της στήλης Β:</t>
-  </si>
-  <si>
-    <t>rt</t>
-  </si>
-  <si>
-    <t>Βαλε στην θεση τα αντιστοιχα συμβολα ( + , - , x , / ) ωστε η πραξει να ειναι ορθη :</t>
-  </si>
-  <si>
-    <t>Βαλε στην θεση τα αντιστοιχα συμβολα ( &lt; , = , &gt; ) ωστε να ειναι ορθα:</t>
-  </si>
-  <si>
-    <t>Βαλε στην αυξουσα σειρα τους παρακατω αριθμους:</t>
-  </si>
-  <si>
-    <t>["1    2   = 3",
-"3    3   =  9",
-"10   2  =  5 ",
-"7     3  =  4"]</t>
-  </si>
-  <si>
-    <t>["+","x","/","-"]</t>
-  </si>
-  <si>
-    <t>["1      3",
-"5      2",
-"10    10",
-"3      9", 
-"7      3"]</t>
-  </si>
-  <si>
-    <t>["&lt;","&gt;","=","&lt;","&gt;"]</t>
-  </si>
-  <si>
-    <t>["1", " 4"," 3," 2","7"," 9","10","8","5","6"]</t>
-  </si>
-  <si>
-    <t>["1","2","3","4","5","6","7","8","9","10"]</t>
+    <t>Σ|Λ</t>
+  </si>
+  <si>
+    <t>Γινόμενο|Πολλαπλασιασμός|Η πράξη με το «x»|Μέθοδος των τριών</t>
+  </si>
+  <si>
+    <t>Οι βαθμοί ενός μαθητή σε 6 μαθήματα ήταν 7, 10, 7, 8, 7, 9. Ο μέσος όρος του θα είναι 8.</t>
+  </si>
+  <si>
+    <t>Μiα παρέα 5 ατόμων μάζεψαν 65 κοχύλια και θέλουν να τα μοιραστούν εξίσου. Άρα το κάθε παιδί θα πάρει 13 κοχύλια.</t>
+  </si>
+  <si>
+    <t>Άθροισμα|Γινόμενο|Διαίρεση|Πηλίκο</t>
+  </si>
+  <si>
+    <t>200|204|198|104</t>
+  </si>
+  <si>
+    <t>9.0|Δεν το έχουμε μάθει|9|3</t>
+  </si>
+  <si>
+    <t>1|3</t>
+  </si>
+  <si>
+    <t>1|4</t>
+  </si>
+  <si>
+    <t>÷ και x|/ και .|÷ και"|/ και *</t>
+  </si>
+  <si>
+    <t>1 και 2|6 και 9|18 και 8|4 και 10</t>
+  </si>
+  <si>
+    <t>Σας δίνονται οι παρακάτω αριθμοί και καλείστε να συμπληρώσετε αν είναι άρτιοι ή περιττοί.</t>
+  </si>
+  <si>
+    <t>57|10|39|31</t>
+  </si>
+  <si>
+    <t>περιττός|άρτιος|περιττός|περιττός</t>
+  </si>
+  <si>
+    <t>Σας δίνονται κάποιες απλές αριθμητικές πράξεις και καλείστε συμπληρώσετε το αποτέλεσμα αυτών των πράξεων.</t>
+  </si>
+  <si>
+    <t>12x3=|20-9=|56+9=|40÷10=</t>
+  </si>
+  <si>
+    <t>36|11|65|4</t>
+  </si>
+  <si>
+    <t>1|2</t>
+  </si>
+  <si>
+    <t>Ποιο είναι το υπόλοιπο των παρακάτω διαιρέσεων;</t>
+  </si>
+  <si>
+    <t>5÷2|8÷8|11÷3|19÷4</t>
+  </si>
+  <si>
+    <t>1|0|2|3</t>
+  </si>
+  <si>
+    <t>Να αντιστοιχίσετε κάθε στοιχείο της δεύτερης στήλης, με ένα στοιχείο της πρώτης στήλης.</t>
+  </si>
+  <si>
+    <t>Πυθαγόρειο|Πρόσθεση|Αφαίρεση!Διαφορά|Θεώρημα|Άθροισμα</t>
+  </si>
+  <si>
+    <t>2|3|1</t>
+  </si>
+  <si>
+    <t>Ποιο είναι το αποτέλεσμα της πράξης 45÷5;</t>
+  </si>
+  <si>
+    <t>Να αντιστοιχήσετε τις πράξεις της δεύτερης στήλης με αυτές της πρώτης στήλης, ώστε να έχουν το ίδιο αποτέλεσμα.</t>
+  </si>
+  <si>
+    <t>10+5=|6-3=|9x3=!9÷3|25-10|15+12</t>
+  </si>
+  <si>
+    <t>2|1|3</t>
+  </si>
+  <si>
+    <t>Να αντιστοιχήσετε τις λέξεις της δεύτερης στήλης, με τα γεωμετρικά σχήματα της πρώτης στήλης.</t>
+  </si>
+  <si>
+    <t>pentagon_path|triangle_path|square_path!Τετράγωνο|Πεντάγωνο|Τρίγωνο</t>
+  </si>
+  <si>
+    <t>3#3=9|1#2=3|10#2=5|7#3=4!+|-|x|÷</t>
+  </si>
+  <si>
+    <t>3|1|4|2</t>
+  </si>
+  <si>
+    <t>Βάλτε στη σωστή θέση τα αντίστοιχα σύμβολα ( + , - , x , ÷ ) , ώστε η πράξη να είναι ορθή.</t>
+  </si>
+  <si>
+    <t>Βάλτε στη σωστή θέση τα αντίστοιχα σύμβολα ( &lt;  , &gt; ) , ώστε να ισχύουν οι ανισότητες.</t>
+  </si>
+  <si>
+    <t>1#3|5#2|3#9|7#3!&lt;|&gt;</t>
+  </si>
+  <si>
+    <t>1|2|1|2</t>
+  </si>
+  <si>
+    <t>Βάλτε σε αύξουσα σειρά τους παρακάτω αριθμούς.</t>
+  </si>
+  <si>
+    <t>1|4|3|2|7|9|10|8|5|6</t>
+  </si>
+  <si>
+    <t>1|2|3|4|5|6|7|8|9|20</t>
+  </si>
+  <si>
+    <t>Πώς λέγεται η πράξη που πραγματοποιείται με το σύμβολο "x";</t>
+  </si>
+  <si>
+    <t>Πώς λέγεται η πράξη που πραγματοποιείται με το σύμβολο "÷";</t>
   </si>
 </sst>
 </file>
@@ -166,10 +195,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -198,7 +229,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -516,92 +547,92 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2837E2A6-D3C0-44EE-8D08-D1968BD1F869}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="117" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" customWidth="1"/>
-    <col min="3" max="3" width="80.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="1"/>
+    <col min="5" max="16384" width="9.08984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="2">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
@@ -613,150 +644,186 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1">
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1">
         <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1">
         <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B11" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="B13" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B14" s="1">
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B15" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B16" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="57.6" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>27</v>
+      <c r="C16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="B17" s="1">
         <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="72" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>28</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="B18" s="1">
         <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>29</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="B19" s="1">
         <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on loading questions.
</commit_message>
<xml_diff>
--- a/Project_final_2022_2023/bin/Debug/net6.0-windows/Questions.xlsx
+++ b/Project_final_2022_2023/bin/Debug/net6.0-windows/Questions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipigr-my.sharepoint.com/personal/p20004_unipi_gr/Documents/Logismiko_Diaxeirishs_Mathishs/Apallaktikh_ergasia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dimit\Desktop\project_final\Project_final_2022_2023\bin\Debug\net6.0-windows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="8_{1B726E18-D274-41B2-BD47-1654DE0783A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AD14668-2AB5-4146-AE70-D0913955CCB2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E065B5E8-A907-426F-A0DA-D2F6A43E160C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-3375" windowWidth="29040" windowHeight="15720" xr2:uid="{8DA8C0F3-3EB6-40DE-8DFC-E7A0383F4D3D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8DA8C0F3-3EB6-40DE-8DFC-E7A0383F4D3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -547,20 +547,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2837E2A6-D3C0-44EE-8D08-D1968BD1F869}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="117" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" customWidth="1"/>
-    <col min="3" max="3" width="80.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.08984375" style="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
         <v>1</v>
       </c>
@@ -574,7 +574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -588,7 +588,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -602,7 +602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -616,7 +616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>46</v>
       </c>
@@ -630,7 +630,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
@@ -644,7 +644,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -658,7 +658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
@@ -672,7 +672,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -686,7 +686,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -700,7 +700,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -714,7 +714,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -728,7 +728,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -742,7 +742,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
@@ -756,7 +756,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>35</v>
       </c>
@@ -770,7 +770,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
@@ -784,7 +784,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>39</v>
       </c>
@@ -798,7 +798,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>40</v>
       </c>
@@ -812,7 +812,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Added questions total time.
</commit_message>
<xml_diff>
--- a/Project_final_2022_2023/bin/Debug/net6.0-windows/Questions.xlsx
+++ b/Project_final_2022_2023/bin/Debug/net6.0-windows/Questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dimit\Desktop\project_final\Project_final_2022_2023\bin\Debug\net6.0-windows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAA0602-BBC5-46CA-9D00-AB55BD7BB723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1C69FF-8405-4A51-85DB-D85CB5835DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-15" windowWidth="29040" windowHeight="15720" xr2:uid="{8DA8C0F3-3EB6-40DE-8DFC-E7A0383F4D3D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{8DA8C0F3-3EB6-40DE-8DFC-E7A0383F4D3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>Type</t>
   </si>
@@ -170,9 +170,6 @@
     <t>1|4|3|2|7|9|10|8|5|6</t>
   </si>
   <si>
-    <t>1|2|3|4|5|6|7|8|9|20</t>
-  </si>
-  <si>
     <t>Πώς λέγεται η πράξη που πραγματοποιείται με το σύμβολο "x";</t>
   </si>
   <si>
@@ -180,6 +177,12 @@
   </si>
   <si>
     <t>Μια παρέα 5 ατόμων μάζεψαν 65 κοχύλια και θέλουν να τα μοιραστούν εξίσου. Άρα το κάθε παιδί θα πάρει 13 κοχύλια.</t>
+  </si>
+  <si>
+    <t>1|2|3|4|5|6|7|8|9|10</t>
+  </si>
+  <si>
+    <t>Duration (sec)</t>
   </si>
 </sst>
 </file>
@@ -545,22 +548,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2837E2A6-D3C0-44EE-8D08-D1968BD1F869}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="117" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" customWidth="1"/>
-    <col min="3" max="3" width="80.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="1"/>
+    <col min="3" max="3" width="73.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.90625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.36328125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2">
         <v>1</v>
       </c>
@@ -573,8 +577,11 @@
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -587,10 +594,13 @@
       <c r="D2" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -601,8 +611,11 @@
       <c r="D3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -615,10 +628,13 @@
       <c r="D4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E4" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -629,10 +645,13 @@
       <c r="D5" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E5" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
@@ -643,8 +662,11 @@
       <c r="D6" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E6" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -657,8 +679,11 @@
       <c r="D7" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E7" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -671,8 +696,11 @@
       <c r="D8" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E8" s="1">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -685,8 +713,11 @@
       <c r="D9" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E9" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -699,8 +730,11 @@
       <c r="D10" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E10" s="1">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -713,8 +747,11 @@
       <c r="D11" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E11" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -727,8 +764,11 @@
       <c r="D12" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E12" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -741,8 +781,11 @@
       <c r="D13" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E13" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -755,8 +798,11 @@
       <c r="D14" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E14" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
@@ -769,8 +815,11 @@
       <c r="D15" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E15" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
@@ -783,8 +832,11 @@
       <c r="D16" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E16" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
@@ -797,8 +849,11 @@
       <c r="D17" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E17" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
@@ -811,8 +866,11 @@
       <c r="D18" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E18" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>42</v>
       </c>
@@ -823,7 +881,10 @@
         <v>43</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
+      </c>
+      <c r="E19" s="1">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Question 4,5 layout completed. Next step: drag and drop, question 5.
</commit_message>
<xml_diff>
--- a/Project_final_2022_2023/bin/Debug/net6.0-windows/Questions.xlsx
+++ b/Project_final_2022_2023/bin/Debug/net6.0-windows/Questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dimit\Desktop\project_final\Project_final_2022_2023\bin\Debug\net6.0-windows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D01908E-E9FE-4939-A907-3D1C3A45F833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0927F3EF-9131-43F8-8B46-24F7F69C0D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8DA8C0F3-3EB6-40DE-8DFC-E7A0383F4D3D}"/>
   </bookViews>
@@ -98,9 +98,6 @@
     <t>Σας δίνονται κάποιες απλές αριθμητικές πράξεις και καλείστε συμπληρώσετε το αποτέλεσμα αυτών των πράξεων.</t>
   </si>
   <si>
-    <t>12x3=|20-9=|56+9=|40÷10=</t>
-  </si>
-  <si>
     <t>36|11|65|4</t>
   </si>
   <si>
@@ -110,9 +107,6 @@
     <t>Ποιο είναι το υπόλοιπο των παρακάτω διαιρέσεων;</t>
   </si>
   <si>
-    <t>5÷2|8÷8|11÷3|19÷4</t>
-  </si>
-  <si>
     <t>1|0|2|3</t>
   </si>
   <si>
@@ -131,9 +125,6 @@
     <t>Να αντιστοιχήσετε τις πράξεις της δεύτερης στήλης με αυτές της πρώτης στήλης, ώστε να έχουν το ίδιο αποτέλεσμα.</t>
   </si>
   <si>
-    <t>10+5=|6-3=|9x3=!9÷3|25-10|15+12</t>
-  </si>
-  <si>
     <t>2|1|3</t>
   </si>
   <si>
@@ -143,9 +134,6 @@
     <t>pentagon_path|triangle_path|square_path!Τετράγωνο|Πεντάγωνο|Τρίγωνο</t>
   </si>
   <si>
-    <t>3#3=9|1#2=3|10#2=5|7#3=4!+|-|x|÷</t>
-  </si>
-  <si>
     <t>3|1|4|2</t>
   </si>
   <si>
@@ -183,6 +171,18 @@
   </si>
   <si>
     <t>÷ και x|/ και .|÷ και "|/ και *</t>
+  </si>
+  <si>
+    <t>12 x 3 =|20 - 9 =|56 + 9 =|40 ÷ 10 =</t>
+  </si>
+  <si>
+    <t>5 ÷ 2 |8 ÷ 8|11 ÷ 3|19 ÷ 4</t>
+  </si>
+  <si>
+    <t>10 + 5 =|6 - 3 =|9 x 3 =!9 ÷ 3 |25 - 10|15 + 12</t>
+  </si>
+  <si>
+    <t>3#3 = 9|1#2 = 3|10#2 = 5|7#3 = 4!+|-|x|÷</t>
   </si>
 </sst>
 </file>
@@ -551,7 +551,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,7 +578,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -600,7 +600,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -634,7 +634,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -651,7 +651,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
@@ -685,7 +685,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1">
         <v>3</v>
@@ -708,7 +708,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>14</v>
@@ -728,7 +728,7 @@
         <v>15</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10" s="1">
         <v>105</v>
@@ -759,10 +759,10 @@
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="E12" s="1">
         <v>120</v>
@@ -770,16 +770,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1">
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E13" s="1">
         <v>120</v>
@@ -787,16 +787,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1">
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E14" s="1">
         <v>60</v>
@@ -804,16 +804,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1">
         <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E15" s="1">
         <v>60</v>
@@ -821,16 +821,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1">
         <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E16" s="1">
         <v>90</v>
@@ -838,16 +838,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B17" s="1">
         <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E17" s="1">
         <v>90</v>
@@ -855,16 +855,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1">
         <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E18" s="1">
         <v>90</v>
@@ -872,16 +872,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B19" s="1">
         <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="E19" s="1">
         <v>90</v>

</xml_diff>

<commit_message>
Fill panels data completed succesfully.
</commit_message>
<xml_diff>
--- a/Project_final_2022_2023/bin/Debug/net6.0-windows/Questions.xlsx
+++ b/Project_final_2022_2023/bin/Debug/net6.0-windows/Questions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dimit\Desktop\project_final\Project_final_2022_2023\bin\Debug\net6.0-windows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0927F3EF-9131-43F8-8B46-24F7F69C0D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C300B99F-7AB4-45BB-8A50-486B1F6B969E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8DA8C0F3-3EB6-40DE-8DFC-E7A0383F4D3D}"/>
   </bookViews>
@@ -149,12 +149,6 @@
     <t>1|2|1|2</t>
   </si>
   <si>
-    <t>Βάλτε σε αύξουσα σειρά τους παρακάτω αριθμούς.</t>
-  </si>
-  <si>
-    <t>1|4|3|2|7|9|10|8|5|6</t>
-  </si>
-  <si>
     <t>Πώς λέγεται η πράξη που πραγματοποιείται με το σύμβολο "x";</t>
   </si>
   <si>
@@ -164,9 +158,6 @@
     <t>Μια παρέα 5 ατόμων μάζεψαν 65 κοχύλια και θέλουν να τα μοιραστούν εξίσου. Άρα το κάθε παιδί θα πάρει 13 κοχύλια.</t>
   </si>
   <si>
-    <t>1|2|3|4|5|6|7|8|9|10</t>
-  </si>
-  <si>
     <t>Duration (sec)</t>
   </si>
   <si>
@@ -183,6 +174,15 @@
   </si>
   <si>
     <t>3#3 = 9|1#2 = 3|10#2 = 5|7#3 = 4!+|-|x|÷</t>
+  </si>
+  <si>
+    <t>1|2|4|5|7|8|10</t>
+  </si>
+  <si>
+    <t>1|4|2|7|10|8|5</t>
+  </si>
+  <si>
+    <t>Βάλτε στη σωστή σειρά τους παρακάτω αριθμούς.</t>
   </si>
 </sst>
 </file>
@@ -550,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2837E2A6-D3C0-44EE-8D08-D1968BD1F869}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,7 +578,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -600,7 +600,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -634,7 +634,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -651,7 +651,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
@@ -708,7 +708,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>14</v>
@@ -759,7 +759,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>20</v>
@@ -776,7 +776,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>23</v>
@@ -827,7 +827,7 @@
         <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>29</v>
@@ -844,7 +844,7 @@
         <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>32</v>
@@ -872,16 +872,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B19" s="1">
         <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E19" s="1">
         <v>90</v>

</xml_diff>